<commit_message>
Refactor long directory and filename in test cases
</commit_message>
<xml_diff>
--- a/diagrams/Long_filepath_deliverable_list.xlsx
+++ b/diagrams/Long_filepath_deliverable_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesse.tsang\Desktop\LongFilepathShorterner\diagrams\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesse\LongFilepathShorterner\diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E83D125-C3F9-44EA-8E04-50399F370C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B09FEA-3B10-4C09-96AF-64F253503E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7EF4DF93-470A-4418-9DBB-08AF649A7756}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{7EF4DF93-470A-4418-9DBB-08AF649A7756}"/>
   </bookViews>
   <sheets>
     <sheet name="Deliverable" sheetId="1" r:id="rId1"/>
@@ -901,23 +901,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96485D63-E1AC-43E1-94C4-0C8B1F518E50}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="103" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="16.5546875" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -946,7 +946,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>7</v>
       </c>
@@ -969,7 +969,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -998,7 +998,7 @@
       </c>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>16</v>
       </c>
@@ -1027,7 +1027,7 @@
       </c>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>18</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>13</v>
       </c>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="I6" s="10"/>
     </row>
-    <row r="7" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>14</v>
       </c>
@@ -1116,7 +1116,7 @@
       </c>
       <c r="I7" s="10"/>
     </row>
-    <row r="8" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>20</v>
       </c>
@@ -1145,7 +1145,7 @@
       </c>
       <c r="I8" s="10"/>
     </row>
-    <row r="9" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>52</v>
       </c>
@@ -1174,7 +1174,7 @@
       </c>
       <c r="I9" s="10"/>
     </row>
-    <row r="10" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>48</v>
       </c>
@@ -1195,13 +1195,13 @@
       </c>
       <c r="I10" s="6"/>
     </row>
-    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>
     </row>
-    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="13"/>
     </row>
-    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="13"/>
     </row>
   </sheetData>
@@ -1214,19 +1214,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E826416-3F19-4B94-8D0F-13E10A4A2432}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="86.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="86.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.109375" customWidth="1"/>
+    <col min="4" max="4" width="64.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="72" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
@@ -1252,7 +1252,7 @@
       </c>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4" ht="54" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
@@ -1264,7 +1264,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" ht="366.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="366.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="72" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>29</v>
       </c>
@@ -1290,7 +1290,7 @@
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" ht="54" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
@@ -1302,7 +1302,7 @@
       </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
@@ -1326,7 +1326,7 @@
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" ht="144" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="150" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>31</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
@@ -1365,14 +1365,14 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="87.109375" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="87.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>59</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="18">
         <v>45320</v>
       </c>
@@ -1392,7 +1392,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="18">
         <v>45321</v>
       </c>
@@ -1401,7 +1401,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="18">
         <v>45322</v>
       </c>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="18">
         <v>45323</v>
       </c>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="18">
         <v>45324</v>
       </c>
@@ -1428,7 +1428,7 @@
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="18">
         <v>45325</v>
       </c>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
         <v>45326</v>
       </c>
@@ -1446,7 +1446,7 @@
       </c>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" ht="108" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="112.5" x14ac:dyDescent="0.3">
       <c r="A9" s="18">
         <v>45327</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="18">
         <v>45328</v>
       </c>
@@ -1466,7 +1466,7 @@
       </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="18">
         <v>45329</v>
       </c>
@@ -1475,7 +1475,7 @@
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="18">
         <v>45330</v>
       </c>
@@ -1484,7 +1484,7 @@
       </c>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="18">
         <v>45331</v>
       </c>
@@ -1493,7 +1493,7 @@
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="18">
         <v>45332</v>
       </c>
@@ -1502,7 +1502,7 @@
       </c>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="18">
         <v>45333</v>
       </c>
@@ -1511,7 +1511,7 @@
       </c>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" ht="29.4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A16" s="18">
         <v>45334</v>
       </c>
@@ -1520,35 +1520,35 @@
       </c>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="18">
         <v>45335</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="18">
         <v>45336</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="18">
         <v>45337</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="18">
         <v>45338</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="18">
         <v>45339</v>
       </c>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="18">
         <v>45340</v>
       </c>
@@ -1566,19 +1566,19 @@
       </c>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="16"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
     </row>
   </sheetData>

</xml_diff>